<commit_message>
fix bugs; optimize (TBD); update performance.xlsx
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -70,10 +70,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MSVC 2017 15.9.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Device: </t>
   </si>
   <si>
@@ -105,10 +101,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PROD-CONS: 1-N: DATAS: 8 bytes * 1000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PROD-CONS: 1-N/N-1/N-N: DATAS: Random 2-256 bytes * 100000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -118,6 +110,14 @@
   </si>
   <si>
     <t>RTT: 293 ms, 2.93 us/d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSVC 2017 15.9.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROD-CONS: 1-N: DATAS: 8 bytes * 10000000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -266,33 +266,57 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$11:$K$18</c:f>
+              <c:f>Sheet1!$K$11:$K$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>9.2285000000000006E-2</c:v>
+                  <c:v>9.0239700000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.101242</c:v>
+                  <c:v>0.117628</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11586200000000001</c:v>
+                  <c:v>0.119631</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13425899999999999</c:v>
+                  <c:v>0.121771</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15809699999999999</c:v>
+                  <c:v>0.121962</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.18026</c:v>
+                  <c:v>0.135294</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.174371</c:v>
+                  <c:v>0.13072300000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.18699399999999999</c:v>
+                  <c:v>0.15015500000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.153367</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15768599999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.160936</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.18023500000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.18453</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.18893799999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.191108</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.21331700000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -327,33 +351,57 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$11:$M$18</c:f>
+              <c:f>Sheet1!$M$11:$M$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>5.6308999999999998E-2</c:v>
+                  <c:v>4.94362E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.4191000000000007E-2</c:v>
+                  <c:v>6.7011200000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.2443999999999998E-2</c:v>
+                  <c:v>8.4845699999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10968600000000001</c:v>
+                  <c:v>0.10240200000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.12783600000000001</c:v>
+                  <c:v>0.121748</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.14316300000000001</c:v>
+                  <c:v>0.13891200000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.18770700000000001</c:v>
+                  <c:v>0.15601300000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25065799999999999</c:v>
+                  <c:v>0.174206</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.19270399999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.20810500000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22763700000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.246616</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26141500000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.28184700000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.29949799999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.31859700000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -369,11 +417,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="77988336"/>
-        <c:axId val="77988896"/>
+        <c:axId val="5694720"/>
+        <c:axId val="5695280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77988336"/>
+        <c:axId val="5694720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -416,7 +464,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77988896"/>
+        <c:crossAx val="5695280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -424,7 +472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77988896"/>
+        <c:axId val="5695280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -475,7 +523,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77988336"/>
+        <c:crossAx val="5694720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -581,7 +629,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$29</c:f>
+              <c:f>Sheet1!$K$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -604,33 +652,57 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$31:$K$38</c:f>
+              <c:f>Sheet1!$K$32:$K$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>2.6113599999999999</c:v>
+                  <c:v>2.6104400000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8805399999999999</c:v>
+                  <c:v>3.0265900000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4303599999999999</c:v>
+                  <c:v>3.10826</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5432899999999998</c:v>
+                  <c:v>3.3552300000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9863900000000001</c:v>
+                  <c:v>3.95919</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.1902200000000001</c:v>
+                  <c:v>3.7821099999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.7573600000000003</c:v>
+                  <c:v>3.6363400000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.9350000000000001</c:v>
+                  <c:v>5.0857599999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.1935399999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.0874499999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0647799999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.8658900000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.8057800000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.7181600000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.7533700000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.2380699999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -642,7 +714,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$29</c:f>
+              <c:f>Sheet1!$M$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -665,33 +737,57 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$31:$M$38</c:f>
+              <c:f>Sheet1!$M$32:$M$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>2.6448299999999998</c:v>
+                  <c:v>2.5075500000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.16181</c:v>
+                  <c:v>2.8048500000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1683500000000002</c:v>
+                  <c:v>3.2104599999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4890699999999999</c:v>
+                  <c:v>3.4733800000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8740899999999998</c:v>
+                  <c:v>3.77041</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.1761200000000001</c:v>
+                  <c:v>4.2278000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.50265</c:v>
+                  <c:v>4.3400299999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.8963700000000001</c:v>
+                  <c:v>4.7204199999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0125000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.36686</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.5405499999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.0112300000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.3065100000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.7450200000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.9313599999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.1775099999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -707,11 +803,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="373889968"/>
-        <c:axId val="373890528"/>
+        <c:axId val="115418688"/>
+        <c:axId val="115419248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="373889968"/>
+        <c:axId val="115418688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -754,7 +850,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373890528"/>
+        <c:crossAx val="115419248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -762,7 +858,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="373890528"/>
+        <c:axId val="115419248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +909,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373889968"/>
+        <c:crossAx val="115418688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -919,7 +1015,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$49</c:f>
+              <c:f>Sheet1!$K$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -942,33 +1038,57 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$51:$K$58</c:f>
+              <c:f>Sheet1!$K$53:$K$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>2.7334299999999998</c:v>
+                  <c:v>2.5648300000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3250500000000001</c:v>
+                  <c:v>2.9794900000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4093200000000001</c:v>
+                  <c:v>3.3267799999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0920500000000004</c:v>
+                  <c:v>3.1336300000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.2398999999999996</c:v>
+                  <c:v>3.6732399999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5070800000000002</c:v>
+                  <c:v>3.81819</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5500400000000001</c:v>
+                  <c:v>3.7398799999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.4633700000000003</c:v>
+                  <c:v>4.0553600000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.2323000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.2150699999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.2405400000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.7354799999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.7111200000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.7540899999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.7960000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.3571499999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -980,7 +1100,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$49</c:f>
+              <c:f>Sheet1!$O$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1003,33 +1123,57 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$51:$O$58</c:f>
+              <c:f>Sheet1!$O$53:$O$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>2.5990000000000002</c:v>
+                  <c:v>2.5153099999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8700100000000002</c:v>
+                  <c:v>2.8775400000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.18872</c:v>
+                  <c:v>3.2767900000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4993500000000002</c:v>
+                  <c:v>3.4444400000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9101499999999998</c:v>
+                  <c:v>3.8282500000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.2172400000000003</c:v>
+                  <c:v>4.1472499999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.5585000000000004</c:v>
+                  <c:v>4.44245</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.8976100000000002</c:v>
+                  <c:v>4.7997800000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.9502899999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4480599999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.7754300000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.9684200000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.3763800000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5753899999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.1476199999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.39194</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1045,11 +1189,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="373893328"/>
-        <c:axId val="373893888"/>
+        <c:axId val="115422048"/>
+        <c:axId val="115422608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="373893328"/>
+        <c:axId val="115422048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,7 +1236,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373893888"/>
+        <c:crossAx val="115422608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1100,7 +1244,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="373893888"/>
+        <c:axId val="115422608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1151,7 +1295,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373893328"/>
+        <c:crossAx val="115422048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1257,7 +1401,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$49</c:f>
+              <c:f>Sheet1!$L$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1280,33 +1424,57 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$51:$L$58</c:f>
+              <c:f>Sheet1!$L$53:$L$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>2.6715300000000002</c:v>
+                  <c:v>2.7715700000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.1226</c:v>
+                  <c:v>10.7324</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.4695</c:v>
+                  <c:v>10.2912</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.7918</c:v>
+                  <c:v>11.4284</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.3848</c:v>
+                  <c:v>11.5778</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.465299999999999</c:v>
+                  <c:v>11.3451</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.053800000000001</c:v>
+                  <c:v>10.704700000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.401</c:v>
+                  <c:v>11.1456</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.715400000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.9465</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.906700000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.6106</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.7377</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.8757000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.880800000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.0069</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1318,7 +1486,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$49</c:f>
+              <c:f>Sheet1!$P$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1341,33 +1509,57 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$51:$P$58</c:f>
+              <c:f>Sheet1!$P$53:$P$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>2.5011899999999998</c:v>
+                  <c:v>2.4991300000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4302299999999999</c:v>
+                  <c:v>2.5253700000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5553499999999998</c:v>
+                  <c:v>2.5178699999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3756399999999998</c:v>
+                  <c:v>2.5294300000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.39785</c:v>
+                  <c:v>2.56351</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.1275000000000004</c:v>
+                  <c:v>2.5523699999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0162199999999997</c:v>
+                  <c:v>2.5636000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.0727500000000001</c:v>
+                  <c:v>2.5693600000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5489899999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5619700000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5632100000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5742099999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.63029</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.61328</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.5856599999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5931199999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1383,11 +1575,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="373896688"/>
-        <c:axId val="373897248"/>
+        <c:axId val="116258320"/>
+        <c:axId val="116258880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="373896688"/>
+        <c:axId val="116258320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1622,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373897248"/>
+        <c:crossAx val="116258880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1438,7 +1630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="373897248"/>
+        <c:axId val="116258880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1489,7 +1681,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373896688"/>
+        <c:crossAx val="116258320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1595,7 +1787,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$49</c:f>
+              <c:f>Sheet1!$M$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1618,33 +1810,57 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$51:$M$58</c:f>
+              <c:f>Sheet1!$M$53:$M$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>2.6688200000000002</c:v>
+                  <c:v>2.6107</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.9112</c:v>
+                  <c:v>8.1776300000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.1748399999999997</c:v>
+                  <c:v>7.5137700000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.4972099999999999</c:v>
+                  <c:v>8.4703599999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1828500000000002</c:v>
+                  <c:v>7.3630300000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.24465</c:v>
+                  <c:v>7.7807500000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5845200000000004</c:v>
+                  <c:v>6.6718400000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.4028799999999997</c:v>
+                  <c:v>4.9131499999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.91378</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9607900000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.98055</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0611800000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0487299999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.1224299999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.1487999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.1454599999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1656,7 +1872,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$49</c:f>
+              <c:f>Sheet1!$Q$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1679,33 +1895,57 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$51:$Q$58</c:f>
+              <c:f>Sheet1!$Q$53:$Q$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>2.5768599999999999</c:v>
+                  <c:v>2.4542899999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5859800000000002</c:v>
+                  <c:v>2.8782000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.1328800000000001</c:v>
+                  <c:v>3.17937</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.4926300000000001</c:v>
+                  <c:v>3.5349200000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.8250500000000001</c:v>
+                  <c:v>3.8344999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.1628600000000002</c:v>
+                  <c:v>4.2059499999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.7853200000000005</c:v>
+                  <c:v>4.5327099999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0521499999999993</c:v>
+                  <c:v>4.8682400000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.1183399999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.48088</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.8329399999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.1995199999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.5546300000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.1986799999999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.1145199999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.4665900000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1721,11 +1961,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="373900048"/>
-        <c:axId val="373900608"/>
+        <c:axId val="116327424"/>
+        <c:axId val="116327984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="373900048"/>
+        <c:axId val="116327424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1768,7 +2008,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373900608"/>
+        <c:crossAx val="116327984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1776,7 +2016,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="373900608"/>
+        <c:axId val="116327984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1827,7 +2067,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373900048"/>
+        <c:crossAx val="116327424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4726,13 +4966,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4758,13 +4998,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4790,13 +5030,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4822,13 +5062,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5116,9 +5356,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q94"/>
+  <dimension ref="A2:Q96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5129,7 +5369,7 @@
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>8</v>
@@ -5140,7 +5380,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>9</v>
@@ -5151,7 +5391,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>10</v>
@@ -5162,7 +5402,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>11</v>
@@ -5173,10 +5413,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -5184,12 +5424,12 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>4</v>
@@ -5203,386 +5443,666 @@
         <v>2</v>
       </c>
       <c r="K11" s="1">
-        <v>9.2285000000000006E-2</v>
+        <v>9.0239700000000006E-2</v>
       </c>
       <c r="M11" s="1">
-        <v>5.6308999999999998E-2</v>
+        <v>4.94362E-2</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="K12" s="1">
-        <v>0.101242</v>
+        <v>0.117628</v>
       </c>
       <c r="M12" s="1">
-        <v>7.4191000000000007E-2</v>
+        <v>6.7011200000000007E-2</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="K13" s="1">
-        <v>0.11586200000000001</v>
+        <v>0.119631</v>
       </c>
       <c r="M13" s="1">
-        <v>9.2443999999999998E-2</v>
+        <v>8.4845699999999996E-2</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="K14" s="1">
-        <v>0.13425899999999999</v>
+        <v>0.121771</v>
       </c>
       <c r="M14" s="1">
-        <v>0.10968600000000001</v>
+        <v>0.10240200000000001</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="K15" s="1">
-        <v>0.15809699999999999</v>
+        <v>0.121962</v>
       </c>
       <c r="M15" s="1">
-        <v>0.12783600000000001</v>
+        <v>0.121748</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="K16" s="1">
-        <v>0.18026</v>
+        <v>0.135294</v>
       </c>
       <c r="M16" s="1">
-        <v>0.14316300000000001</v>
+        <v>0.13891200000000001</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="K17" s="1">
-        <v>0.174371</v>
+        <v>0.13072300000000001</v>
       </c>
       <c r="M17" s="1">
-        <v>0.18770700000000001</v>
+        <v>0.15601300000000001</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="K18" s="1">
-        <v>0.18699399999999999</v>
+        <v>0.15015500000000001</v>
       </c>
       <c r="M18" s="1">
-        <v>0.25065799999999999</v>
+        <v>0.174206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K19" s="1">
+        <v>0.153367</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0.19270399999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K20" s="1">
+        <v>0.15768599999999999</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0.20810500000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K21" s="1">
+        <v>0.160936</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0.22763700000000001</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="J22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B27" s="1" t="s">
-        <v>0</v>
+      <c r="K22" s="2">
+        <v>0.18023500000000001</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0.246616</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K23" s="1">
+        <v>0.18453</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0.26141500000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K24" s="1">
+        <v>0.18893799999999999</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0.28184700000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K25" s="1">
+        <v>0.191108</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0.29949799999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K26" s="1">
+        <v>0.21331700000000001</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0.31859700000000002</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K29" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="M30" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K31" s="1">
-        <v>2.6113599999999999</v>
-      </c>
-      <c r="M31" s="1">
-        <v>2.6448299999999998</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
       <c r="K32" s="1">
-        <v>2.8805399999999999</v>
+        <v>2.6104400000000001</v>
       </c>
       <c r="M32" s="1">
-        <v>3.16181</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.15">
+        <v>2.5075500000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="10:13" x14ac:dyDescent="0.15">
       <c r="K33" s="1">
-        <v>3.4303599999999999</v>
+        <v>3.0265900000000001</v>
       </c>
       <c r="M33" s="1">
-        <v>3.1683500000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.15">
+        <v>2.8048500000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="10:13" x14ac:dyDescent="0.15">
       <c r="K34" s="1">
-        <v>3.5432899999999998</v>
+        <v>3.10826</v>
       </c>
       <c r="M34" s="1">
-        <v>3.4890699999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.15">
+        <v>3.2104599999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="10:13" x14ac:dyDescent="0.15">
       <c r="K35" s="1">
-        <v>3.9863900000000001</v>
+        <v>3.3552300000000002</v>
       </c>
       <c r="M35" s="1">
-        <v>3.8740899999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.15">
+        <v>3.4733800000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="10:13" x14ac:dyDescent="0.15">
       <c r="K36" s="1">
-        <v>4.1902200000000001</v>
+        <v>3.95919</v>
       </c>
       <c r="M36" s="1">
-        <v>4.1761200000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.15">
+        <v>3.77041</v>
+      </c>
+    </row>
+    <row r="37" spans="10:13" x14ac:dyDescent="0.15">
       <c r="K37" s="1">
-        <v>4.7573600000000003</v>
+        <v>3.7821099999999999</v>
       </c>
       <c r="M37" s="1">
-        <v>4.50265</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.15">
+        <v>4.2278000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="10:13" x14ac:dyDescent="0.15">
       <c r="K38" s="1">
-        <v>3.9350000000000001</v>
+        <v>3.6363400000000001</v>
       </c>
       <c r="M38" s="1">
-        <v>4.8963700000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="J42" s="3" t="s">
+        <v>4.3400299999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="10:13" x14ac:dyDescent="0.15">
+      <c r="K39" s="1">
+        <v>5.0857599999999996</v>
+      </c>
+      <c r="M39" s="1">
+        <v>4.7204199999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="10:13" x14ac:dyDescent="0.15">
+      <c r="K40" s="1">
+        <v>4.1935399999999996</v>
+      </c>
+      <c r="M40" s="1">
+        <v>5.0125000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="10:13" x14ac:dyDescent="0.15">
+      <c r="K41" s="1">
+        <v>4.0874499999999996</v>
+      </c>
+      <c r="M41" s="1">
+        <v>5.36686</v>
+      </c>
+    </row>
+    <row r="42" spans="10:13" x14ac:dyDescent="0.15">
+      <c r="K42" s="1">
+        <v>4.0647799999999998</v>
+      </c>
+      <c r="M42" s="1">
+        <v>5.5405499999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="10:13" x14ac:dyDescent="0.15">
+      <c r="J43" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K42" s="2"/>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B47" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B48" s="1" t="s">
-        <v>23</v>
+      <c r="K43" s="2">
+        <v>4.8658900000000003</v>
+      </c>
+      <c r="M43" s="1">
+        <v>6.0112300000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="10:13" x14ac:dyDescent="0.15">
+      <c r="K44" s="1">
+        <v>4.8057800000000004</v>
+      </c>
+      <c r="M44" s="1">
+        <v>6.3065100000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="10:13" x14ac:dyDescent="0.15">
+      <c r="K45" s="1">
+        <v>4.7181600000000001</v>
+      </c>
+      <c r="M45" s="1">
+        <v>6.7450200000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="10:13" x14ac:dyDescent="0.15">
+      <c r="K46" s="1">
+        <v>4.7533700000000003</v>
+      </c>
+      <c r="M46" s="1">
+        <v>6.9313599999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="10:13" x14ac:dyDescent="0.15">
+      <c r="K47" s="1">
+        <v>5.2380699999999996</v>
+      </c>
+      <c r="M47" s="1">
+        <v>7.1775099999999998</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K49" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="B50" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="B51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="L51" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M49" s="1" t="s">
+      <c r="M51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O49" s="1" t="s">
+      <c r="O51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P49" s="1" t="s">
+      <c r="P51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q51" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q49" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A51" s="3" t="s">
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K51" s="1">
-        <v>2.7334299999999998</v>
-      </c>
-      <c r="L51" s="1">
-        <v>2.6715300000000002</v>
-      </c>
-      <c r="M51" s="1">
-        <v>2.6688200000000002</v>
-      </c>
-      <c r="O51" s="1">
-        <v>2.5990000000000002</v>
-      </c>
-      <c r="P51" s="1">
-        <v>2.5011899999999998</v>
-      </c>
-      <c r="Q51" s="1">
-        <v>2.5768599999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="K52" s="1">
-        <v>3.3250500000000001</v>
-      </c>
-      <c r="L52" s="1">
-        <v>10.1226</v>
-      </c>
-      <c r="M52" s="1">
-        <v>7.9112</v>
-      </c>
-      <c r="O52" s="1">
-        <v>2.8700100000000002</v>
-      </c>
-      <c r="P52" s="1">
-        <v>4.4302299999999999</v>
-      </c>
-      <c r="Q52" s="1">
-        <v>5.5859800000000002</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K53" s="1">
-        <v>3.4093200000000001</v>
+        <v>2.5648300000000002</v>
       </c>
       <c r="L53" s="1">
-        <v>11.4695</v>
+        <v>2.7715700000000001</v>
       </c>
       <c r="M53" s="1">
-        <v>6.1748399999999997</v>
+        <v>2.6107</v>
       </c>
       <c r="O53" s="1">
-        <v>3.18872</v>
+        <v>2.5153099999999999</v>
       </c>
       <c r="P53" s="1">
-        <v>4.5553499999999998</v>
+        <v>2.4991300000000001</v>
       </c>
       <c r="Q53" s="1">
-        <v>6.1328800000000001</v>
+        <v>2.4542899999999999</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K54" s="1">
-        <v>4.0920500000000004</v>
+        <v>2.9794900000000002</v>
       </c>
       <c r="L54" s="1">
-        <v>10.7918</v>
+        <v>10.7324</v>
       </c>
       <c r="M54" s="1">
-        <v>5.4972099999999999</v>
+        <v>8.1776300000000006</v>
       </c>
       <c r="O54" s="1">
-        <v>3.4993500000000002</v>
+        <v>2.8775400000000002</v>
       </c>
       <c r="P54" s="1">
-        <v>4.3756399999999998</v>
+        <v>2.5253700000000001</v>
       </c>
       <c r="Q54" s="1">
-        <v>6.4926300000000001</v>
+        <v>2.8782000000000001</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K55" s="1">
-        <v>4.2398999999999996</v>
+        <v>3.3267799999999998</v>
       </c>
       <c r="L55" s="1">
-        <v>11.3848</v>
+        <v>10.2912</v>
       </c>
       <c r="M55" s="1">
-        <v>5.1828500000000002</v>
+        <v>7.5137700000000001</v>
       </c>
       <c r="O55" s="1">
-        <v>3.9101499999999998</v>
+        <v>3.2767900000000001</v>
       </c>
       <c r="P55" s="1">
-        <v>4.39785</v>
+        <v>2.5178699999999998</v>
       </c>
       <c r="Q55" s="1">
-        <v>6.8250500000000001</v>
+        <v>3.17937</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K56" s="1">
-        <v>3.5070800000000002</v>
+        <v>3.1336300000000001</v>
       </c>
       <c r="L56" s="1">
-        <v>11.465299999999999</v>
+        <v>11.4284</v>
       </c>
       <c r="M56" s="1">
-        <v>5.24465</v>
+        <v>8.4703599999999994</v>
       </c>
       <c r="O56" s="1">
-        <v>4.2172400000000003</v>
+        <v>3.4444400000000002</v>
       </c>
       <c r="P56" s="1">
-        <v>4.1275000000000004</v>
+        <v>2.5294300000000001</v>
       </c>
       <c r="Q56" s="1">
-        <v>7.1628600000000002</v>
+        <v>3.5349200000000001</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K57" s="1">
-        <v>3.5500400000000001</v>
+        <v>3.6732399999999998</v>
       </c>
       <c r="L57" s="1">
-        <v>11.053800000000001</v>
+        <v>11.5778</v>
       </c>
       <c r="M57" s="1">
-        <v>5.5845200000000004</v>
+        <v>7.3630300000000002</v>
       </c>
       <c r="O57" s="1">
-        <v>4.5585000000000004</v>
+        <v>3.8282500000000002</v>
       </c>
       <c r="P57" s="1">
-        <v>5.0162199999999997</v>
+        <v>2.56351</v>
       </c>
       <c r="Q57" s="1">
-        <v>8.7853200000000005</v>
+        <v>3.8344999999999998</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K58" s="1">
-        <v>4.4633700000000003</v>
+        <v>3.81819</v>
       </c>
       <c r="L58" s="1">
-        <v>11.401</v>
+        <v>11.3451</v>
       </c>
       <c r="M58" s="1">
-        <v>6.4028799999999997</v>
+        <v>7.7807500000000003</v>
       </c>
       <c r="O58" s="1">
-        <v>4.8976100000000002</v>
+        <v>4.1472499999999997</v>
       </c>
       <c r="P58" s="1">
-        <v>4.0727500000000001</v>
+        <v>2.5523699999999998</v>
       </c>
       <c r="Q58" s="1">
-        <v>8.0521499999999993</v>
+        <v>4.2059499999999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="K59" s="1">
+        <v>3.7398799999999999</v>
+      </c>
+      <c r="L59" s="1">
+        <v>10.704700000000001</v>
+      </c>
+      <c r="M59" s="1">
+        <v>6.6718400000000004</v>
+      </c>
+      <c r="O59" s="1">
+        <v>4.44245</v>
+      </c>
+      <c r="P59" s="1">
+        <v>2.5636000000000001</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>4.5327099999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="K60" s="1">
+        <v>4.0553600000000003</v>
+      </c>
+      <c r="L60" s="1">
+        <v>11.1456</v>
+      </c>
+      <c r="M60" s="1">
+        <v>4.9131499999999999</v>
+      </c>
+      <c r="O60" s="1">
+        <v>4.7997800000000002</v>
+      </c>
+      <c r="P60" s="1">
+        <v>2.5693600000000001</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>4.8682400000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="K61" s="1">
+        <v>4.2323000000000004</v>
+      </c>
+      <c r="L61" s="1">
+        <v>10.715400000000001</v>
+      </c>
+      <c r="M61" s="1">
+        <v>4.91378</v>
+      </c>
+      <c r="O61" s="1">
+        <v>4.9502899999999999</v>
+      </c>
+      <c r="P61" s="1">
+        <v>2.5489899999999999</v>
+      </c>
+      <c r="Q61" s="1">
+        <v>5.1183399999999999</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="J62" s="3" t="s">
+      <c r="K62" s="1">
+        <v>6.2150699999999999</v>
+      </c>
+      <c r="L62" s="1">
+        <v>10.9465</v>
+      </c>
+      <c r="M62" s="1">
+        <v>4.9607900000000003</v>
+      </c>
+      <c r="O62" s="1">
+        <v>5.4480599999999999</v>
+      </c>
+      <c r="P62" s="1">
+        <v>2.5619700000000001</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>5.48088</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="K63" s="1">
+        <v>4.2405400000000002</v>
+      </c>
+      <c r="L63" s="1">
+        <v>10.906700000000001</v>
+      </c>
+      <c r="M63" s="1">
+        <v>4.98055</v>
+      </c>
+      <c r="O63" s="1">
+        <v>5.7754300000000001</v>
+      </c>
+      <c r="P63" s="1">
+        <v>2.5632100000000002</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>5.8329399999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="J64" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A67" s="3" t="s">
+      <c r="K64" s="1">
+        <v>4.7354799999999999</v>
+      </c>
+      <c r="L64" s="1">
+        <v>10.6106</v>
+      </c>
+      <c r="M64" s="1">
+        <v>5.0611800000000002</v>
+      </c>
+      <c r="O64" s="1">
+        <v>5.9684200000000001</v>
+      </c>
+      <c r="P64" s="1">
+        <v>2.5742099999999999</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>6.1995199999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="K65" s="1">
+        <v>4.7111200000000002</v>
+      </c>
+      <c r="L65" s="1">
+        <v>10.7377</v>
+      </c>
+      <c r="M65" s="1">
+        <v>5.0487299999999999</v>
+      </c>
+      <c r="O65" s="1">
+        <v>6.3763800000000002</v>
+      </c>
+      <c r="P65" s="1">
+        <v>2.63029</v>
+      </c>
+      <c r="Q65" s="1">
+        <v>6.5546300000000004</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="K66" s="1">
+        <v>4.7540899999999997</v>
+      </c>
+      <c r="L66" s="1">
+        <v>9.8757000000000001</v>
+      </c>
+      <c r="M66" s="1">
+        <v>5.1224299999999996</v>
+      </c>
+      <c r="O66" s="1">
+        <v>6.5753899999999996</v>
+      </c>
+      <c r="P66" s="1">
+        <v>2.61328</v>
+      </c>
+      <c r="Q66" s="1">
+        <v>8.1986799999999995</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="K67" s="1">
+        <v>4.7960000000000003</v>
+      </c>
+      <c r="L67" s="1">
+        <v>10.880800000000001</v>
+      </c>
+      <c r="M67" s="1">
+        <v>5.1487999999999996</v>
+      </c>
+      <c r="O67" s="1">
+        <v>7.1476199999999999</v>
+      </c>
+      <c r="P67" s="1">
+        <v>2.5856599999999998</v>
+      </c>
+      <c r="Q67" s="1">
+        <v>7.1145199999999997</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="K68" s="1">
+        <v>5.3571499999999999</v>
+      </c>
+      <c r="L68" s="1">
+        <v>11.0069</v>
+      </c>
+      <c r="M68" s="1">
+        <v>5.1454599999999999</v>
+      </c>
+      <c r="O68" s="1">
+        <v>7.39194</v>
+      </c>
+      <c r="P68" s="1">
+        <v>2.5931199999999999</v>
+      </c>
+      <c r="Q68" s="1">
+        <v>7.4665900000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A69" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="J78" s="3" t="s">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="J80" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A83" s="3" t="s">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A85" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="J94" s="3" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="J96" s="3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modify test cases of mem; sync_pool_alloc => async_pool_alloc, synchronized => async_wrapper; statical => static_wrapper; optimize ipc::mem::allocator; use std::hardware_destructive_interference_size for cache_line_size (TBD); simplified codes.
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\MyFiles\cpp-ipc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.91.133\dev\cpp-ipc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06F5F70-6343-475F-9C1A-823BA46B779E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ipc" sheetId="1" r:id="rId1"/>
+    <sheet name="alloc" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t>ipc::route</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -120,11 +122,50 @@
     <t>RTT: 243.364 ms, 2.43364 us/d</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>24 GB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMD Ryzen™ 5 1400 @ 3.2 GHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ubuntu 18.04.2 Server x64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g++ v7.4.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSI B450M MORTAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Mainboard: </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>static_alloc</t>
+  </si>
+  <si>
+    <t>pool_alloc</t>
+  </si>
+  <si>
+    <t>alloc_FIFO</t>
+  </si>
+  <si>
+    <t>alloc_LIFO</t>
+  </si>
+  <si>
+    <t>alloc_random</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -219,7 +260,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -243,7 +284,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$9</c:f>
+              <c:f>ipc!$K$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -266,7 +307,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$11:$K$26</c:f>
+              <c:f>ipc!$K$11:$K$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -322,13 +363,18 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8973-4194-8AF6-AF6177EA20AB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$9</c:f>
+              <c:f>ipc!$M$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -351,7 +397,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$11:$M$26</c:f>
+              <c:f>ipc!$M$11:$M$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -407,6 +453,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8973-4194-8AF6-AF6177EA20AB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -537,7 +588,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -605,7 +655,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -629,7 +679,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$30</c:f>
+              <c:f>ipc!$K$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -652,7 +702,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$32:$K$47</c:f>
+              <c:f>ipc!$K$32:$K$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -708,13 +758,18 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE1B-4E3E-BC0C-859ACE388F1D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$30</c:f>
+              <c:f>ipc!$M$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -737,7 +792,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$32:$M$47</c:f>
+              <c:f>ipc!$M$32:$M$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -793,6 +848,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FE1B-4E3E-BC0C-859ACE388F1D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -923,7 +983,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -991,7 +1050,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -1015,7 +1074,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$51</c:f>
+              <c:f>ipc!$K$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1038,7 +1097,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$53:$K$68</c:f>
+              <c:f>ipc!$K$53:$K$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1094,13 +1153,18 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F542-43F9-92A6-1B25A8265977}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$51</c:f>
+              <c:f>ipc!$O$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1123,7 +1187,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$53:$O$68</c:f>
+              <c:f>ipc!$O$53:$O$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1179,6 +1243,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F542-43F9-92A6-1B25A8265977}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1309,7 +1378,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1377,7 +1445,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -1401,7 +1469,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$51</c:f>
+              <c:f>ipc!$L$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1424,7 +1492,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$53:$L$68</c:f>
+              <c:f>ipc!$L$53:$L$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1480,13 +1548,18 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-04F4-4959-B13D-9D7E101B0BE4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$51</c:f>
+              <c:f>ipc!$P$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1509,7 +1582,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$53:$P$68</c:f>
+              <c:f>ipc!$P$53:$P$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1565,6 +1638,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-04F4-4959-B13D-9D7E101B0BE4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1695,7 +1773,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1763,7 +1840,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -1787,7 +1864,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$51</c:f>
+              <c:f>ipc!$M$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1824,7 +1901,7 @@
           </c:trendline>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$53:$M$68</c:f>
+              <c:f>ipc!$M$53:$M$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1880,13 +1957,18 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2E9F-4DB8-BBDE-A544A1834DD5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$51</c:f>
+              <c:f>ipc!$Q$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1923,7 +2005,7 @@
           </c:trendline>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$53:$Q$68</c:f>
+              <c:f>ipc!$Q$53:$Q$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1979,6 +2061,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2E9F-4DB8-BBDE-A544A1834DD5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2109,7 +2196,1047 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>alloc!$K$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>static_alloc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>alloc!$K$11:$K$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6.5199199999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9909600000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0792999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3684199999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9681800000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.76137E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4991899999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.4993000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F29C-4CFB-90CA-C0F28EF86A94}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>alloc!$M$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pool_alloc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>alloc!$M$11:$M$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.2804500000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2472799999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9042700000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4363300000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1745899999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8879799999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7452100000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6038400000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F29C-4CFB-90CA-C0F28EF86A94}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="233353920"/>
+        <c:axId val="233354480"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="233353920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233354480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="233354480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233353920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>alloc!$K$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>static_alloc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>alloc!$K$30:$K$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.119547</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.39102E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.81901E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0432700000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1586499999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.9997400000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.69477E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.6167499999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F3FC-4205-8335-AE76CA6DE20E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>alloc!$M$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pool_alloc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>alloc!$M$30:$M$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.7120799999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9845500000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0585599999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8076499999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7373E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5765399999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4528599999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.35902E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F3FC-4205-8335-AE76CA6DE20E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="233357280"/>
+        <c:axId val="233357840"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="233357280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233357840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="233357840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233357280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>alloc!$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>static_alloc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>alloc!$K$49:$K$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.45289099999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.252334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17851</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16103300000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.144926</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13439599999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.130052</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.12673699999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7B5F-48DD-BC52-95FBE0BEBCF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>alloc!$M$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pool_alloc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>alloc!$M$49:$M$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.39221600000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.220193</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16481999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14047799999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11862399999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.111821</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.105632</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7B5F-48DD-BC52-95FBE0BEBCF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="233357280"/>
+        <c:axId val="233357840"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="233357280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233357840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="233357840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233357280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2376,6 +3503,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4441,6 +5688,1554 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4973,7 +7768,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="图表 2"/>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5005,7 +7806,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="图表 3"/>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5037,7 +7844,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="图表 4"/>
+        <xdr:cNvPr id="5" name="图表 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5069,7 +7882,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="图表 6"/>
+        <xdr:cNvPr id="7" name="图表 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5101,7 +7920,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="图表 7"/>
+        <xdr:cNvPr id="8" name="图表 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5113,6 +7938,125 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E4C7510-9276-4E9C-99D0-B868E8DA9AC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF31C86B-6813-4764-8C02-EC9B6DB314F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96DDA0AA-D18C-412C-9769-05EE24077CDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5383,7 +8327,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -6140,4 +9084,317 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{663AD7C5-3B96-48B2-9E43-5815C75C304F}">
+  <dimension ref="A2:M56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="10.625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1">
+        <v>6.5199199999999999E-2</v>
+      </c>
+      <c r="M11" s="1">
+        <v>8.2804500000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K12" s="1">
+        <v>6.9909600000000002E-2</v>
+      </c>
+      <c r="M12" s="1">
+        <v>4.2472799999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K13" s="1">
+        <v>5.0792999999999998E-2</v>
+      </c>
+      <c r="M13" s="1">
+        <v>2.9042700000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K14" s="1">
+        <v>4.3684199999999999E-2</v>
+      </c>
+      <c r="M14" s="1">
+        <v>2.4363300000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K15" s="1">
+        <v>3.9681800000000003E-2</v>
+      </c>
+      <c r="M15" s="1">
+        <v>2.1745899999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K16" s="1">
+        <v>3.76137E-2</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1.8879799999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K17" s="1">
+        <v>3.4991899999999999E-2</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1.7452100000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K18" s="1">
+        <v>3.4993000000000003E-2</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1.6038400000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K22" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0.119547</v>
+      </c>
+      <c r="M30" s="1">
+        <v>5.7120799999999999E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K31" s="1">
+        <v>6.39102E-2</v>
+      </c>
+      <c r="M31" s="1">
+        <v>2.9845500000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K32" s="1">
+        <v>4.81901E-2</v>
+      </c>
+      <c r="M32" s="1">
+        <v>2.0585599999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="K33" s="1">
+        <v>4.0432700000000002E-2</v>
+      </c>
+      <c r="M33" s="1">
+        <v>1.8076499999999999E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="K34" s="1">
+        <v>4.1586499999999998E-2</v>
+      </c>
+      <c r="M34" s="1">
+        <v>1.7373E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="K35" s="1">
+        <v>3.9997400000000002E-2</v>
+      </c>
+      <c r="M35" s="1">
+        <v>1.5765399999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="K36" s="1">
+        <v>3.69477E-2</v>
+      </c>
+      <c r="M36" s="1">
+        <v>1.4528599999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="K37" s="1">
+        <v>3.6167499999999998E-2</v>
+      </c>
+      <c r="M37" s="1">
+        <v>1.35902E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B47" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A49" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K49" s="1">
+        <v>0.45289099999999999</v>
+      </c>
+      <c r="M49" s="1">
+        <v>0.39221600000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K50" s="1">
+        <v>0.252334</v>
+      </c>
+      <c r="M50" s="1">
+        <v>0.220193</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K51" s="1">
+        <v>0.17851</v>
+      </c>
+      <c r="M51" s="1">
+        <v>0.16481999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K52" s="1">
+        <v>0.16103300000000001</v>
+      </c>
+      <c r="M52" s="1">
+        <v>0.14047799999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K53" s="1">
+        <v>0.144926</v>
+      </c>
+      <c r="M53" s="1">
+        <v>0.12997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K54" s="1">
+        <v>0.13439599999999999</v>
+      </c>
+      <c r="M54" s="1">
+        <v>0.11862399999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K55" s="1">
+        <v>0.130052</v>
+      </c>
+      <c r="M55" s="1">
+        <v>0.111821</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="K56" s="1">
+        <v>0.12673699999999999</v>
+      </c>
+      <c r="M56" s="1">
+        <v>0.105632</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
optimize the memory allocator
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.91.133\dev\cpp-ipc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.91.128\dev\cpp-ipc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D12126-FA64-48EF-A34F-19A63C034C72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C4D612-C00D-43A8-8A5F-6382AD094D36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -887,28 +887,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>22.4101</c:v>
+                  <c:v>18.213799999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.4999300000000009</c:v>
+                  <c:v>9.2019199999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.12378</c:v>
+                  <c:v>5.9444400000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3043800000000001</c:v>
+                  <c:v>4.3105900000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0059100000000001</c:v>
+                  <c:v>4.28071</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.80931</c:v>
+                  <c:v>4.2800799999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.8460799999999997</c:v>
+                  <c:v>4.2952500000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9590699999999996</c:v>
+                  <c:v>3.6126200000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1402,28 +1402,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.117186</c:v>
+                  <c:v>0.134765</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.99108E-2</c:v>
+                  <c:v>7.0637199999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.03201E-2</c:v>
+                  <c:v>7.4726600000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2389600000000001E-2</c:v>
+                  <c:v>6.8225900000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.7184900000000002E-2</c:v>
+                  <c:v>3.8167E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4759500000000003E-2</c:v>
+                  <c:v>5.1627600000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.7545700000000001E-2</c:v>
+                  <c:v>4.8516299999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.5044600000000003E-2</c:v>
+                  <c:v>4.0766700000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1918,28 +1918,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.12839900000000001</c:v>
+                  <c:v>0.116756</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.2871E-2</c:v>
+                  <c:v>6.7525399999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.4259799999999997E-2</c:v>
+                  <c:v>6.9706000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2673299999999999E-2</c:v>
+                  <c:v>8.3218600000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.32737E-2</c:v>
+                  <c:v>9.35111E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9114999999999997E-2</c:v>
+                  <c:v>3.8509399999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.9312800000000003E-2</c:v>
+                  <c:v>3.6715999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0288200000000001E-2</c:v>
+                  <c:v>3.3855400000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2434,28 +2434,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.23471500000000001</c:v>
+                  <c:v>0.25068299999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.159576</c:v>
+                  <c:v>0.15091099999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9034300000000006E-2</c:v>
+                  <c:v>9.8360500000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0255000000000007E-2</c:v>
+                  <c:v>0.106714</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.70948E-2</c:v>
+                  <c:v>0.101275</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.12750300000000001</c:v>
+                  <c:v>8.2291100000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13981199999999999</c:v>
+                  <c:v>9.0575199999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.104946</c:v>
+                  <c:v>0.11984300000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4555,28 +4555,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>20.6556</c:v>
+                  <c:v>17.9376</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.2623999999999995</c:v>
+                  <c:v>9.2064299999999992</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.7915599999999996</c:v>
+                  <c:v>5.2313700000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2144500000000003</c:v>
+                  <c:v>4.1915399999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0107499999999998</c:v>
+                  <c:v>4.2234100000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.6699799999999998</c:v>
+                  <c:v>4.1966999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6478700000000002</c:v>
+                  <c:v>4.1783900000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.7900299999999998</c:v>
+                  <c:v>3.3681899999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5070,28 +5070,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>9.5208200000000007E-2</c:v>
+                  <c:v>0.104979</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9800900000000002E-2</c:v>
+                  <c:v>5.2007400000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4472700000000002E-2</c:v>
+                  <c:v>5.3499499999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0235499999999998E-2</c:v>
+                  <c:v>4.2333799999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9458999999999999E-2</c:v>
+                  <c:v>4.4232599999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.8426399999999999E-2</c:v>
+                  <c:v>4.5316000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.6670200000000002E-2</c:v>
+                  <c:v>4.7363500000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5007499999999997E-2</c:v>
+                  <c:v>3.6313499999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5586,28 +5586,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>8.9974600000000002E-2</c:v>
+                  <c:v>8.88901E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.2315500000000001E-2</c:v>
+                  <c:v>4.7537599999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5381099999999999E-2</c:v>
+                  <c:v>3.8765399999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0585500000000002E-2</c:v>
+                  <c:v>4.0281999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9272099999999999E-2</c:v>
+                  <c:v>3.6654899999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.67248E-2</c:v>
+                  <c:v>3.9388199999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.28464E-2</c:v>
+                  <c:v>3.4458599999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.6997299999999998E-2</c:v>
+                  <c:v>2.8533200000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6102,28 +6102,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.22829199999999999</c:v>
+                  <c:v>0.25519999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14486199999999999</c:v>
+                  <c:v>0.147202</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.106833</c:v>
+                  <c:v>9.2210799999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.6607900000000007E-2</c:v>
+                  <c:v>9.4175099999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.7924300000000002E-2</c:v>
+                  <c:v>0.100257</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.6098400000000005E-2</c:v>
+                  <c:v>0.103667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.1250000000000003E-2</c:v>
+                  <c:v>9.55091E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.6041499999999998E-2</c:v>
+                  <c:v>9.1973299999999994E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15287,7 +15287,7 @@
         <v>10.541600000000001</v>
       </c>
       <c r="O12" s="10">
-        <v>20.6556</v>
+        <v>17.9376</v>
       </c>
       <c r="Q12" s="1">
         <v>8.6701700000000006</v>
@@ -15301,7 +15301,7 @@
         <v>5.3596599999999999</v>
       </c>
       <c r="O13" s="10">
-        <v>9.2623999999999995</v>
+        <v>9.2064299999999992</v>
       </c>
       <c r="Q13" s="1">
         <v>4.5791199999999996</v>
@@ -15315,7 +15315,7 @@
         <v>3.5325299999999999</v>
       </c>
       <c r="O14" s="10">
-        <v>6.7915599999999996</v>
+        <v>5.2313700000000001</v>
       </c>
       <c r="Q14" s="1">
         <v>3.6274299999999999</v>
@@ -15329,7 +15329,7 @@
         <v>2.6282000000000001</v>
       </c>
       <c r="O15" s="10">
-        <v>5.2144500000000003</v>
+        <v>4.1915399999999998</v>
       </c>
       <c r="Q15" s="1">
         <v>2.5146199999999999</v>
@@ -15343,7 +15343,7 @@
         <v>2.5251000000000001</v>
       </c>
       <c r="O16" s="10">
-        <v>5.0107499999999998</v>
+        <v>4.2234100000000003</v>
       </c>
       <c r="Q16" s="1">
         <v>2.4251299999999998</v>
@@ -15357,7 +15357,7 @@
         <v>2.5264000000000002</v>
       </c>
       <c r="O17" s="10">
-        <v>4.6699799999999998</v>
+        <v>4.1966999999999999</v>
       </c>
       <c r="Q17" s="1">
         <v>2.10771</v>
@@ -15371,7 +15371,7 @@
         <v>2.6773199999999999</v>
       </c>
       <c r="O18" s="10">
-        <v>4.6478700000000002</v>
+        <v>4.1783900000000003</v>
       </c>
       <c r="Q18" s="1">
         <v>1.9367000000000001</v>
@@ -15385,7 +15385,7 @@
         <v>2.5134500000000002</v>
       </c>
       <c r="O19" s="10">
-        <v>4.7900299999999998</v>
+        <v>3.3681899999999998</v>
       </c>
       <c r="Q19" s="1">
         <v>1.9221699999999999</v>
@@ -15422,7 +15422,7 @@
         <v>10.231299999999999</v>
       </c>
       <c r="O34" s="10">
-        <v>22.4101</v>
+        <v>18.213799999999999</v>
       </c>
       <c r="Q34" s="7">
         <v>8.7434100000000008</v>
@@ -15433,7 +15433,7 @@
         <v>5.2037199999999997</v>
       </c>
       <c r="O35" s="10">
-        <v>9.4999300000000009</v>
+        <v>9.2019199999999994</v>
       </c>
       <c r="Q35" s="7">
         <v>4.4105299999999996</v>
@@ -15444,7 +15444,7 @@
         <v>3.1685599999999998</v>
       </c>
       <c r="O36" s="10">
-        <v>7.12378</v>
+        <v>5.9444400000000002</v>
       </c>
       <c r="Q36" s="7">
         <v>2.41486</v>
@@ -15455,7 +15455,7 @@
         <v>2.5904500000000001</v>
       </c>
       <c r="O37" s="10">
-        <v>5.3043800000000001</v>
+        <v>4.3105900000000004</v>
       </c>
       <c r="Q37" s="7">
         <v>1.82796</v>
@@ -15466,7 +15466,7 @@
         <v>2.6365400000000001</v>
       </c>
       <c r="O38" s="10">
-        <v>5.0059100000000001</v>
+        <v>4.28071</v>
       </c>
       <c r="Q38" s="7">
         <v>1.86852</v>
@@ -15477,7 +15477,7 @@
         <v>2.4535800000000001</v>
       </c>
       <c r="O39" s="10">
-        <v>4.80931</v>
+        <v>4.2800799999999999</v>
       </c>
       <c r="Q39" s="7">
         <v>1.8126800000000001</v>
@@ -15488,7 +15488,7 @@
         <v>2.5073300000000001</v>
       </c>
       <c r="O40" s="10">
-        <v>4.8460799999999997</v>
+        <v>4.2952500000000002</v>
       </c>
       <c r="Q40" s="7">
         <v>1.7874399999999999</v>
@@ -15499,7 +15499,7 @@
         <v>2.48143</v>
       </c>
       <c r="O41" s="10">
-        <v>4.9590699999999996</v>
+        <v>3.6126200000000002</v>
       </c>
       <c r="Q41" s="7">
         <v>1.88551</v>
@@ -15568,7 +15568,7 @@
         <v>0.126358</v>
       </c>
       <c r="O58" s="10">
-        <v>9.5208200000000007E-2</v>
+        <v>0.104979</v>
       </c>
       <c r="Q58" s="1">
         <v>8.0589099999999997E-2</v>
@@ -15579,7 +15579,7 @@
         <v>0.46383099999999999</v>
       </c>
       <c r="O59" s="10">
-        <v>4.9800900000000002E-2</v>
+        <v>5.2007400000000002E-2</v>
       </c>
       <c r="Q59" s="1">
         <v>3.8287599999999998E-2</v>
@@ -15590,7 +15590,7 @@
         <v>0.43428299999999997</v>
       </c>
       <c r="O60" s="10">
-        <v>3.4472700000000002E-2</v>
+        <v>5.3499499999999998E-2</v>
       </c>
       <c r="Q60" s="1">
         <v>3.37451E-2</v>
@@ -15601,7 +15601,7 @@
         <v>0.46758499999999997</v>
       </c>
       <c r="O61" s="10">
-        <v>3.0235499999999998E-2</v>
+        <v>4.2333799999999998E-2</v>
       </c>
       <c r="Q61" s="1">
         <v>3.8703899999999999E-2</v>
@@ -15612,7 +15612,7 @@
         <v>0.230075</v>
       </c>
       <c r="O62" s="10">
-        <v>2.9458999999999999E-2</v>
+        <v>4.4232599999999997E-2</v>
       </c>
       <c r="Q62" s="1">
         <v>3.8491999999999998E-2</v>
@@ -15623,7 +15623,7 @@
         <v>0.17593700000000001</v>
       </c>
       <c r="O63" s="10">
-        <v>3.8426399999999999E-2</v>
+        <v>4.5316000000000002E-2</v>
       </c>
       <c r="Q63" s="1">
         <v>3.7897100000000003E-2</v>
@@ -15634,7 +15634,7 @@
         <v>6.2992800000000002E-2</v>
       </c>
       <c r="O64" s="10">
-        <v>2.6670200000000002E-2</v>
+        <v>4.7363500000000003E-2</v>
       </c>
       <c r="Q64" s="1">
         <v>3.4671100000000003E-2</v>
@@ -15645,7 +15645,7 @@
         <v>6.0430999999999999E-2</v>
       </c>
       <c r="O65" s="10">
-        <v>3.5007499999999997E-2</v>
+        <v>3.6313499999999999E-2</v>
       </c>
       <c r="Q65" s="1">
         <v>3.8071199999999999E-2</v>
@@ -15664,7 +15664,7 @@
         <v>0.26969900000000002</v>
       </c>
       <c r="O80" s="10">
-        <v>0.117186</v>
+        <v>0.134765</v>
       </c>
       <c r="Q80" s="1">
         <v>8.2161899999999996E-2</v>
@@ -15675,7 +15675,7 @@
         <v>1.5039199999999999</v>
       </c>
       <c r="O81" s="10">
-        <v>5.99108E-2</v>
+        <v>7.0637199999999997E-2</v>
       </c>
       <c r="Q81" s="1">
         <v>6.3500899999999999E-2</v>
@@ -15686,7 +15686,7 @@
         <v>2.3091499999999998</v>
       </c>
       <c r="O82" s="10">
-        <v>5.03201E-2</v>
+        <v>7.4726600000000004E-2</v>
       </c>
       <c r="Q82" s="1">
         <v>6.3998200000000005E-2</v>
@@ -15697,7 +15697,7 @@
         <v>1.8403799999999999</v>
       </c>
       <c r="O83" s="10">
-        <v>5.2389600000000001E-2</v>
+        <v>6.8225900000000006E-2</v>
       </c>
       <c r="Q83" s="1">
         <v>8.2786999999999999E-2</v>
@@ -15708,7 +15708,7 @@
         <v>0.92615199999999998</v>
       </c>
       <c r="O84" s="10">
-        <v>4.7184900000000002E-2</v>
+        <v>3.8167E-2</v>
       </c>
       <c r="Q84" s="1">
         <v>8.2739400000000005E-2</v>
@@ -15719,7 +15719,7 @@
         <v>0.45206600000000002</v>
       </c>
       <c r="O85" s="10">
-        <v>5.4759500000000003E-2</v>
+        <v>5.1627600000000003E-2</v>
       </c>
       <c r="Q85" s="1">
         <v>6.9639699999999999E-2</v>
@@ -15730,7 +15730,7 @@
         <v>0.105153</v>
       </c>
       <c r="O86" s="10">
-        <v>3.7545700000000001E-2</v>
+        <v>4.8516299999999998E-2</v>
       </c>
       <c r="Q86" s="1">
         <v>4.2977799999999997E-2</v>
@@ -15741,7 +15741,7 @@
         <v>5.7405499999999998E-2</v>
       </c>
       <c r="O87" s="10">
-        <v>7.5044600000000003E-2</v>
+        <v>4.0766700000000003E-2</v>
       </c>
       <c r="Q87" s="1">
         <v>5.9599399999999997E-2</v>
@@ -15774,7 +15774,7 @@
         <v>0.123201</v>
       </c>
       <c r="O104" s="10">
-        <v>8.9974600000000002E-2</v>
+        <v>8.88901E-2</v>
       </c>
       <c r="Q104" s="1">
         <v>5.7443899999999999E-2</v>
@@ -15785,7 +15785,7 @@
         <v>0.15046799999999999</v>
       </c>
       <c r="O105" s="10">
-        <v>5.2315500000000001E-2</v>
+        <v>4.7537599999999999E-2</v>
       </c>
       <c r="Q105" s="1">
         <v>4.8631399999999998E-2</v>
@@ -15796,7 +15796,7 @@
         <v>0.39644800000000002</v>
       </c>
       <c r="O106" s="10">
-        <v>3.5381099999999999E-2</v>
+        <v>3.8765399999999998E-2</v>
       </c>
       <c r="Q106" s="1">
         <v>3.7522100000000003E-2</v>
@@ -15807,7 +15807,7 @@
         <v>0.31692799999999999</v>
       </c>
       <c r="O107" s="10">
-        <v>3.0585500000000002E-2</v>
+        <v>4.0281999999999998E-2</v>
       </c>
       <c r="Q107" s="1">
         <v>3.64757E-2</v>
@@ -15818,7 +15818,7 @@
         <v>0.12166299999999999</v>
       </c>
       <c r="O108" s="10">
-        <v>2.9272099999999999E-2</v>
+        <v>3.6654899999999997E-2</v>
       </c>
       <c r="Q108" s="1">
         <v>3.6965400000000002E-2</v>
@@ -15829,7 +15829,7 @@
         <v>9.7332500000000002E-2</v>
       </c>
       <c r="O109" s="10">
-        <v>2.67248E-2</v>
+        <v>3.9388199999999998E-2</v>
       </c>
       <c r="Q109" s="1">
         <v>3.4648900000000003E-2</v>
@@ -15840,7 +15840,7 @@
         <v>7.5878600000000004E-2</v>
       </c>
       <c r="O110" s="10">
-        <v>4.28464E-2</v>
+        <v>3.4458599999999999E-2</v>
       </c>
       <c r="Q110" s="1">
         <v>3.7302299999999997E-2</v>
@@ -15851,7 +15851,7 @@
         <v>6.6806299999999999E-2</v>
       </c>
       <c r="O111" s="10">
-        <v>2.6997299999999998E-2</v>
+        <v>2.8533200000000002E-2</v>
       </c>
       <c r="Q111" s="1">
         <v>3.4824800000000003E-2</v>
@@ -15867,7 +15867,7 @@
         <v>0.279505</v>
       </c>
       <c r="O126" s="10">
-        <v>0.12839900000000001</v>
+        <v>0.116756</v>
       </c>
       <c r="Q126" s="1">
         <v>7.6657799999999998E-2</v>
@@ -15879,7 +15879,7 @@
         <v>1.9100200000000001</v>
       </c>
       <c r="O127" s="10">
-        <v>8.2871E-2</v>
+        <v>6.7525399999999999E-2</v>
       </c>
       <c r="Q127" s="1">
         <v>7.1522199999999994E-2</v>
@@ -15890,7 +15890,7 @@
         <v>2.1775699999999998</v>
       </c>
       <c r="O128" s="10">
-        <v>5.4259799999999997E-2</v>
+        <v>6.9706000000000004E-2</v>
       </c>
       <c r="Q128" s="1">
         <v>6.6224099999999994E-2</v>
@@ -15901,7 +15901,7 @@
         <v>1.7882800000000001</v>
       </c>
       <c r="O129" s="10">
-        <v>5.2673299999999999E-2</v>
+        <v>8.3218600000000004E-2</v>
       </c>
       <c r="Q129" s="1">
         <v>6.7210699999999998E-2</v>
@@ -15912,7 +15912,7 @@
         <v>0.142404</v>
       </c>
       <c r="O130" s="10">
-        <v>5.32737E-2</v>
+        <v>9.35111E-2</v>
       </c>
       <c r="Q130" s="1">
         <v>6.5678600000000004E-2</v>
@@ -15923,7 +15923,7 @@
         <v>0.419354</v>
       </c>
       <c r="O131" s="10">
-        <v>3.9114999999999997E-2</v>
+        <v>3.8509399999999999E-2</v>
       </c>
       <c r="Q131" s="1">
         <v>6.6912700000000006E-2</v>
@@ -15934,7 +15934,7 @@
         <v>4.5165999999999998E-2</v>
       </c>
       <c r="O132" s="10">
-        <v>7.9312800000000003E-2</v>
+        <v>3.6715999999999999E-2</v>
       </c>
       <c r="Q132" s="1">
         <v>5.4892999999999997E-2</v>
@@ -15945,7 +15945,7 @@
         <v>4.4523699999999999E-2</v>
       </c>
       <c r="O133" s="10">
-        <v>3.0288200000000001E-2</v>
+        <v>3.3855400000000001E-2</v>
       </c>
       <c r="Q133" s="1">
         <v>7.2250400000000006E-2</v>
@@ -15978,7 +15978,7 @@
         <v>0.45372000000000001</v>
       </c>
       <c r="O150" s="10">
-        <v>0.22829199999999999</v>
+        <v>0.25519999999999998</v>
       </c>
       <c r="Q150" s="1">
         <v>0.256276</v>
@@ -15989,7 +15989,7 @@
         <v>0.27060499999999998</v>
       </c>
       <c r="O151" s="10">
-        <v>0.14486199999999999</v>
+        <v>0.147202</v>
       </c>
       <c r="Q151" s="1">
         <v>0.16822899999999999</v>
@@ -16000,7 +16000,7 @@
         <v>0.18004999999999999</v>
       </c>
       <c r="O152" s="10">
-        <v>0.106833</v>
+        <v>9.2210799999999996E-2</v>
       </c>
       <c r="Q152" s="1">
         <v>0.102316</v>
@@ -16011,7 +16011,7 @@
         <v>0.14088400000000001</v>
       </c>
       <c r="O153" s="10">
-        <v>7.6607900000000007E-2</v>
+        <v>9.4175099999999998E-2</v>
       </c>
       <c r="Q153" s="1">
         <v>7.4685600000000005E-2</v>
@@ -16022,7 +16022,7 @@
         <v>0.248502</v>
       </c>
       <c r="O154" s="10">
-        <v>7.7924300000000002E-2</v>
+        <v>0.100257</v>
       </c>
       <c r="Q154" s="1">
         <v>7.0671300000000006E-2</v>
@@ -16033,7 +16033,7 @@
         <v>0.17857300000000001</v>
       </c>
       <c r="O155" s="10">
-        <v>8.6098400000000005E-2</v>
+        <v>0.103667</v>
       </c>
       <c r="Q155" s="1">
         <v>6.9693599999999994E-2</v>
@@ -16044,7 +16044,7 @@
         <v>0.12940199999999999</v>
       </c>
       <c r="O156" s="10">
-        <v>8.1250000000000003E-2</v>
+        <v>9.55091E-2</v>
       </c>
       <c r="Q156" s="1">
         <v>7.06508E-2</v>
@@ -16055,7 +16055,7 @@
         <v>0.111954</v>
       </c>
       <c r="O157" s="10">
-        <v>7.6041499999999998E-2</v>
+        <v>9.1973299999999994E-2</v>
       </c>
       <c r="Q157" s="1">
         <v>7.7969999999999998E-2</v>
@@ -16071,7 +16071,7 @@
         <v>0.53479399999999999</v>
       </c>
       <c r="O172" s="10">
-        <v>0.23471500000000001</v>
+        <v>0.25068299999999999</v>
       </c>
       <c r="Q172" s="1">
         <v>0.23760800000000001</v>
@@ -16083,7 +16083,7 @@
         <v>0.70010499999999998</v>
       </c>
       <c r="O173" s="10">
-        <v>0.159576</v>
+        <v>0.15091099999999999</v>
       </c>
       <c r="Q173" s="1">
         <v>0.143094</v>
@@ -16094,7 +16094,7 @@
         <v>1.4507699999999999</v>
       </c>
       <c r="O174" s="10">
-        <v>9.9034300000000006E-2</v>
+        <v>9.8360500000000003E-2</v>
       </c>
       <c r="Q174" s="1">
         <v>8.7562100000000004E-2</v>
@@ -16105,7 +16105,7 @@
         <v>1.43197</v>
       </c>
       <c r="O175" s="10">
-        <v>8.0255000000000007E-2</v>
+        <v>0.106714</v>
       </c>
       <c r="Q175" s="1">
         <v>8.8886300000000001E-2</v>
@@ -16116,7 +16116,7 @@
         <v>0.42857499999999998</v>
       </c>
       <c r="O176" s="10">
-        <v>8.70948E-2</v>
+        <v>0.101275</v>
       </c>
       <c r="Q176" s="1">
         <v>9.7954299999999994E-2</v>
@@ -16127,7 +16127,7 @@
         <v>0.12822900000000001</v>
       </c>
       <c r="O177" s="10">
-        <v>0.12750300000000001</v>
+        <v>8.2291100000000006E-2</v>
       </c>
       <c r="Q177" s="1">
         <v>9.2671400000000001E-2</v>
@@ -16138,7 +16138,7 @@
         <v>7.1667700000000001E-2</v>
       </c>
       <c r="O178" s="10">
-        <v>0.13981199999999999</v>
+        <v>9.0575199999999995E-2</v>
       </c>
       <c r="Q178" s="1">
         <v>8.2737900000000003E-2</v>
@@ -16149,7 +16149,7 @@
         <v>7.5734099999999999E-2</v>
       </c>
       <c r="O179" s="10">
-        <v>0.104946</v>
+        <v>0.11984300000000001</v>
       </c>
       <c r="Q179" s="1">
         <v>8.7262599999999996E-2</v>

</xml_diff>